<commit_message>
Add setup.py; full pipeline running
</commit_message>
<xml_diff>
--- a/mg_template.xlsx
+++ b/mg_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-4100" yWindow="-20040" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="1680" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>mg_f</t>
   </si>
@@ -33,9 +33,6 @@
     <t>/mnt/stepanauskas_nfs/julia/testfragrecruitment/hmp/illumina_mgs/SRS019030/SRS019030.denovo_duplicates_marked.trimmed.1.fastq.gz</t>
   </si>
   <si>
-    <t>/mnt/stepanauskas_nfs/julia/testfragrecruitment/hmp/illumina_mgs/SRS019030/SRS019030.denovo_duplicates_marked.trimmed.2.fastq.gz</t>
-  </si>
-  <si>
     <t>illumina</t>
   </si>
   <si>
@@ -45,21 +42,6 @@
     <t>/mnt/stepanauskas_nfs/julia/testfragrecruitment/hmp/illumina_mgs/SRS078197/SRS078197.denovo_duplicates_marked.trimmed.1.fastq.gz</t>
   </si>
   <si>
-    <t>/mnt/stepanauskas_nfs/julia/testfragrecruitment/hmp/illumina_mgs/SRS022524/SRS022524.denovo_duplicates_marked.trimmed.2.fastq.gz</t>
-  </si>
-  <si>
-    <t>/mnt/stepanauskas_nfs/julia/testfragrecruitment/hmp/illumina_mgs/SRS078197/SRS078197.denovo_duplicates_marked.trimmed.2.fastq.gz</t>
-  </si>
-  <si>
-    <t>/mnt/stepanauskas_nfs/julia/testfragrecruitment/hmp/pyro_mgs/SRS019030_454/SRR063559.fastq.gz</t>
-  </si>
-  <si>
-    <t>/mnt/stepanauskas_nfs/julia/testfragrecruitment/hmp/pyro_mgs/SRS078197_454/SRR061736.fastq.gz</t>
-  </si>
-  <si>
-    <t>/mnt/stepanauskas_nfs/julia/testfragrecruitment/hmp/pyro_mgs/SRS022524_454/SRR063903.fastq.gz</t>
-  </si>
-  <si>
     <t>pyro</t>
   </si>
   <si>
@@ -67,6 +49,15 @@
   </si>
   <si>
     <t>join</t>
+  </si>
+  <si>
+    <t>/mnt/stepanauskas_nfs/julia/testfragrecruitment/hmp/pyro_mgs/SRS019030_454/SRS019030_454.fastq.gz</t>
+  </si>
+  <si>
+    <t>/mnt/stepanauskas_nfs/julia/testfragrecruitment/hmp/pyro_mgs/SRS022524_454/SRS022524_45.fastq.gz</t>
+  </si>
+  <si>
+    <t>/mnt/stepanauskas_nfs/julia/testfragrecruitment/hmp/pyro_mgs/SRS078197_454/SRS078197_454.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -466,13 +457,13 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="116.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -486,7 +477,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -494,41 +485,41 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -536,10 +527,10 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -547,13 +538,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -561,13 +552,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
more search terms to mask sag
also added try, except to join reads step
</commit_message>
<xml_diff>
--- a/mg_template.xlsx
+++ b/mg_template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>mg_f</t>
   </si>
@@ -30,34 +30,19 @@
     <t>wgs_technology</t>
   </si>
   <si>
-    <t>/mnt/stepanauskas_nfs/julia/testfragrecruitment/hmp/illumina_mgs/SRS019030/SRS019030.denovo_duplicates_marked.trimmed.1.fastq.gz</t>
-  </si>
-  <si>
     <t>illumina</t>
   </si>
   <si>
-    <t>/mnt/stepanauskas_nfs/julia/testfragrecruitment/hmp/illumina_mgs/SRS022524/SRS022524.denovo_duplicates_marked.trimmed.1.fastq.gz</t>
-  </si>
-  <si>
-    <t>/mnt/stepanauskas_nfs/julia/testfragrecruitment/hmp/illumina_mgs/SRS078197/SRS078197.denovo_duplicates_marked.trimmed.1.fastq.gz</t>
-  </si>
-  <si>
-    <t>pyro</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
     <t>join</t>
   </si>
   <si>
-    <t>/mnt/stepanauskas_nfs/julia/testfragrecruitment/hmp/pyro_mgs/SRS019030_454/SRS019030_454.fastq.gz</t>
-  </si>
-  <si>
-    <t>/mnt/stepanauskas_nfs/julia/testfragrecruitment/hmp/pyro_mgs/SRS022524_454/SRS022524_45.fastq.gz</t>
-  </si>
-  <si>
-    <t>/mnt/stepanauskas_nfs/julia/testfragrecruitment/hmp/pyro_mgs/SRS078197_454/SRS078197_454.fastq.gz</t>
+    <t>/mnt/stepanauskas_nfs/ebecraft/OV2_metagenome/OV-2_P2_metagenome.fastq</t>
+  </si>
+  <si>
+    <t>/mnt/stepanauskas_nfs/ebecraft/OV2_metagenome/OV-2_P3_metagenome.fastq</t>
   </si>
 </sst>
 </file>
@@ -106,8 +91,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -118,13 +105,15 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -454,11 +443,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -477,91 +464,35 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
       <c r="D2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
name column added to mg table
</commit_message>
<xml_diff>
--- a/mg_template.xlsx
+++ b/mg_template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>mg_f</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>/mnt/stepanauskas_nfs/ebecraft/OV2_metagenome/OV-2_P3_metagenome.fastq</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>OV-2_P2_metagenome</t>
+  </si>
+  <si>
+    <t>OV-2_P3_metagenome</t>
   </si>
 </sst>
 </file>
@@ -443,55 +452,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="116.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="b">
+      <c r="E2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="b">
+      <c r="E3" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>